<commit_message>
create localhost folder and database script
</commit_message>
<xml_diff>
--- a/00. Document/00. Database/Database_Define.xlsx
+++ b/00. Document/00. Database/Database_Define.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="122">
   <si>
     <t>Table name</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Bruiser</t>
   </si>
   <si>
-    <t>2015.0.1</t>
-  </si>
-  <si>
     <t>T01ChampRole</t>
   </si>
   <si>
@@ -381,6 +378,12 @@
   </si>
   <si>
     <t>atk_range_incr</t>
+  </si>
+  <si>
+    <t>updatetime</t>
+  </si>
+  <si>
+    <t>long</t>
   </si>
 </sst>
 </file>
@@ -947,7 +950,7 @@
   <dimension ref="A2:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +969,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1056,13 +1059,13 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="G8" t="s">
-        <v>21</v>
+      <c r="G8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1124,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1147,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1155,7 +1158,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -1201,7 +1204,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1209,18 +1212,18 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1228,18 +1231,18 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,20 +1250,20 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1268,20 +1271,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1289,20 +1292,20 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1310,18 +1313,18 @@
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1329,16 +1332,16 @@
         <v>8</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5" t="s">
@@ -1350,16 +1353,16 @@
         <v>9</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5" t="s">
@@ -1371,16 +1374,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="5">
         <v>0</v>
@@ -1394,16 +1397,16 @@
         <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="F16" s="5">
         <v>0</v>
@@ -1417,16 +1420,16 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="F17" s="5">
         <v>0</v>
@@ -1440,16 +1443,16 @@
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
@@ -1463,14 +1466,14 @@
         <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
@@ -1484,14 +1487,14 @@
         <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
@@ -1505,18 +1508,18 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,7 +1530,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>13</v>
@@ -1538,8 +1541,8 @@
       <c r="F22" s="5">
         <v>0</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>21</v>
+      <c r="G22" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1587,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1610,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -1618,7 +1621,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -1664,7 +1667,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1672,20 +1675,20 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1693,16 +1696,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -1716,16 +1719,16 @@
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
@@ -1739,16 +1742,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -1762,16 +1765,16 @@
         <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -1785,16 +1788,16 @@
         <v>7</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -1808,16 +1811,16 @@
         <v>8</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -1831,16 +1834,16 @@
         <v>9</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
@@ -1854,16 +1857,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="F15" s="5">
         <v>0</v>
@@ -1877,16 +1880,16 @@
         <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F16" s="5">
         <v>0</v>
@@ -1900,16 +1903,16 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" s="5">
         <v>0</v>
@@ -1923,16 +1926,16 @@
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
@@ -1946,16 +1949,16 @@
         <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
@@ -1969,16 +1972,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
@@ -1992,16 +1995,16 @@
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="F21" s="5">
         <v>0</v>
@@ -2015,16 +2018,16 @@
         <v>17</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
         <v>100</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>101</v>
       </c>
       <c r="F22" s="5">
         <v>0</v>
@@ -2038,16 +2041,16 @@
         <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="F23" s="5">
         <v>0</v>
@@ -2061,16 +2064,16 @@
         <v>19</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="F24" s="5">
         <v>0</v>
@@ -2084,16 +2087,16 @@
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="F25" s="5">
         <v>0</v>
@@ -2107,16 +2110,16 @@
         <v>21</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="F26" s="5">
         <v>0</v>
@@ -2130,16 +2133,16 @@
         <v>22</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="F27" s="5">
         <v>0</v>
@@ -2156,17 +2159,17 @@
         <v>15</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="5" t="s">
-        <v>21</v>
+      <c r="G28" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2223,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G10:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2246,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -2254,7 +2257,7 @@
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -2300,7 +2303,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2308,20 +2311,20 @@
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2329,27 +2332,35 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="4">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>

</xml_diff>